<commit_message>
Ordené el script, cambié nombres de algunas variables, agregué una mejor forma de escribir la comparación.
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Milagros Azcueta\Documents\GitHub\TP-FINAL-BIOME\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive - cnba.uba.ar\UBA\Biologia\Biometría II\TP-FINAL-BIOME\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16111CD-0E45-42A1-BDD1-399DAC5ACCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11232"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sin muertos + Sin 0" sheetId="4" r:id="rId1"/>
@@ -45,9 +46,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Semana</t>
-  </si>
-  <si>
     <t>ANT</t>
   </si>
   <si>
@@ -80,11 +78,14 @@
   <si>
     <t>TRATAMIENTO</t>
   </si>
+  <si>
+    <t>SEMANA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -281,7 +282,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -356,6 +357,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -391,6 +409,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -566,73 +601,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="1" customWidth="1"/>
-    <col min="10" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="4.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="6.88671875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.44140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.6640625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.44140625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.33203125" style="1" customWidth="1"/>
-    <col min="26" max="28" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.33203125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
+    <col min="10" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="4.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="5.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.85546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.42578125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.28515625" style="1" customWidth="1"/>
+    <col min="26" max="28" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.28515625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.7109375" style="1" customWidth="1"/>
     <col min="31" max="31" width="4" style="1" customWidth="1"/>
-    <col min="32" max="32" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="44" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="12.109375" style="1" customWidth="1"/>
-    <col min="48" max="48" width="6.88671875" style="1" customWidth="1"/>
-    <col min="49" max="49" width="7.109375" style="1" customWidth="1"/>
-    <col min="50" max="50" width="8.88671875" style="1" customWidth="1"/>
-    <col min="51" max="51" width="7.6640625" style="1" customWidth="1"/>
-    <col min="52" max="52" width="8.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.88671875" style="1" customWidth="1"/>
-    <col min="54" max="55" width="9.44140625" style="1" customWidth="1"/>
-    <col min="56" max="56" width="8.6640625" style="1" customWidth="1"/>
-    <col min="57" max="57" width="7.6640625" style="1" customWidth="1"/>
-    <col min="58" max="60" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="61" max="1013" width="12.109375" style="1" customWidth="1"/>
-    <col min="1014" max="16384" width="11.44140625" style="1"/>
+    <col min="32" max="32" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="44" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="12.140625" style="1" customWidth="1"/>
+    <col min="48" max="48" width="6.85546875" style="1" customWidth="1"/>
+    <col min="49" max="49" width="7.140625" style="1" customWidth="1"/>
+    <col min="50" max="50" width="8.85546875" style="1" customWidth="1"/>
+    <col min="51" max="51" width="7.7109375" style="1" customWidth="1"/>
+    <col min="52" max="52" width="8.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.85546875" style="1" customWidth="1"/>
+    <col min="54" max="55" width="9.42578125" style="1" customWidth="1"/>
+    <col min="56" max="56" width="8.7109375" style="1" customWidth="1"/>
+    <col min="57" max="57" width="7.7109375" style="1" customWidth="1"/>
+    <col min="58" max="60" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="1013" width="12.140625" style="1" customWidth="1"/>
+    <col min="1014" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>10</v>
-      </c>
       <c r="E1" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>0</v>
@@ -657,7 +692,7 @@
       </c>
       <c r="M1" s="8"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -665,13 +700,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="6">
         <v>0</v>
@@ -696,7 +731,7 @@
       </c>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -704,13 +739,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="6">
         <v>0</v>
@@ -735,7 +770,7 @@
       </c>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -743,13 +778,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="6">
         <v>0</v>
@@ -774,7 +809,7 @@
       </c>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>1</v>
       </c>
@@ -782,13 +817,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="6">
         <v>0</v>
@@ -813,7 +848,7 @@
       </c>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>1</v>
       </c>
@@ -821,13 +856,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="6">
         <v>0</v>
@@ -852,7 +887,7 @@
       </c>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>1</v>
       </c>
@@ -860,13 +895,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="7">
         <v>0</v>
@@ -891,7 +926,7 @@
       </c>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>1</v>
       </c>
@@ -899,13 +934,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="6">
         <v>0</v>
@@ -930,7 +965,7 @@
       </c>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>1</v>
       </c>
@@ -938,13 +973,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="6">
         <v>0</v>
@@ -969,7 +1004,7 @@
       </c>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>1</v>
       </c>
@@ -977,13 +1012,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="6">
         <v>0</v>
@@ -1008,7 +1043,7 @@
       </c>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>1</v>
       </c>
@@ -1016,14 +1051,14 @@
         <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F11" s="6">
         <v>0</v>
       </c>
@@ -1047,7 +1082,7 @@
       </c>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>1</v>
       </c>
@@ -1055,14 +1090,14 @@
         <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F12" s="6">
         <v>0</v>
       </c>
@@ -1086,7 +1121,7 @@
       </c>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>1</v>
       </c>
@@ -1094,14 +1129,14 @@
         <v>12</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F13" s="6">
         <v>0</v>
       </c>
@@ -1125,7 +1160,7 @@
       </c>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>1</v>
       </c>
@@ -1133,14 +1168,14 @@
         <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F14" s="6">
         <v>0</v>
       </c>
@@ -1164,7 +1199,7 @@
       </c>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>1</v>
       </c>
@@ -1172,14 +1207,14 @@
         <v>14</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F15" s="6">
         <v>0</v>
       </c>
@@ -1203,7 +1238,7 @@
       </c>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>1</v>
       </c>
@@ -1211,14 +1246,14 @@
         <v>15</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F16" s="6">
         <v>0</v>
       </c>
@@ -1242,7 +1277,7 @@
       </c>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>1</v>
       </c>
@@ -1250,14 +1285,14 @@
         <v>16</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F17" s="6">
         <v>0</v>
       </c>
@@ -1281,7 +1316,7 @@
       </c>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>1</v>
       </c>
@@ -1289,13 +1324,13 @@
         <v>17</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F18" s="6">
         <v>0</v>
@@ -1320,7 +1355,7 @@
       </c>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>1</v>
       </c>
@@ -1328,13 +1363,13 @@
         <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" s="6">
         <v>0</v>
@@ -1359,7 +1394,7 @@
       </c>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>1</v>
       </c>
@@ -1367,13 +1402,13 @@
         <v>19</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F20" s="6">
         <v>0</v>
@@ -1398,7 +1433,7 @@
       </c>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>1</v>
       </c>
@@ -1406,13 +1441,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F21" s="7">
         <v>0</v>
@@ -1437,7 +1472,7 @@
       </c>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>1</v>
       </c>
@@ -1445,13 +1480,13 @@
         <v>21</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F22" s="6">
         <v>0</v>
@@ -1476,7 +1511,7 @@
       </c>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>2</v>
       </c>
@@ -1484,13 +1519,13 @@
         <v>22</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F23" s="6">
         <v>0</v>
@@ -1515,7 +1550,7 @@
       </c>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>2</v>
       </c>
@@ -1523,13 +1558,13 @@
         <v>23</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" s="6">
         <v>0</v>
@@ -1554,7 +1589,7 @@
       </c>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>2</v>
       </c>
@@ -1562,13 +1597,13 @@
         <v>24</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F25" s="6">
         <v>0</v>
@@ -1593,7 +1628,7 @@
       </c>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>2</v>
       </c>
@@ -1601,13 +1636,13 @@
         <v>25</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26" s="6">
         <v>0</v>
@@ -1632,7 +1667,7 @@
       </c>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>2</v>
       </c>
@@ -1640,13 +1675,13 @@
         <v>26</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F27" s="6">
         <v>0</v>
@@ -1671,7 +1706,7 @@
       </c>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>2</v>
       </c>
@@ -1679,13 +1714,13 @@
         <v>27</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F28" s="6">
         <v>0</v>
@@ -1710,7 +1745,7 @@
       </c>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>2</v>
       </c>
@@ -1718,14 +1753,14 @@
         <v>28</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F29" s="7">
         <v>0</v>
       </c>
@@ -1749,7 +1784,7 @@
       </c>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>2</v>
       </c>
@@ -1757,14 +1792,14 @@
         <v>29</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F30" s="7">
         <v>0</v>
       </c>
@@ -1788,7 +1823,7 @@
       </c>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>2</v>
       </c>
@@ -1796,14 +1831,14 @@
         <v>30</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F31" s="6">
         <v>0</v>
       </c>
@@ -1827,7 +1862,7 @@
       </c>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>2</v>
       </c>
@@ -1835,14 +1870,14 @@
         <v>31</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F32" s="6">
         <v>0</v>
       </c>
@@ -1866,7 +1901,7 @@
       </c>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>2</v>
       </c>
@@ -1874,14 +1909,14 @@
         <v>32</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F33" s="6">
         <v>0</v>
       </c>
@@ -1905,7 +1940,7 @@
       </c>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>2</v>
       </c>
@@ -1913,13 +1948,13 @@
         <v>33</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F34" s="6">
         <v>0</v>
@@ -1944,7 +1979,7 @@
       </c>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>2</v>
       </c>
@@ -1952,13 +1987,13 @@
         <v>34</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F35" s="6">
         <v>0</v>
@@ -1983,7 +2018,7 @@
       </c>
       <c r="M35" s="2"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>3</v>
       </c>
@@ -1991,13 +2026,13 @@
         <v>35</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F36" s="6">
         <v>0</v>
@@ -2022,7 +2057,7 @@
       </c>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>3</v>
       </c>
@@ -2030,13 +2065,13 @@
         <v>36</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F37" s="7">
         <v>0</v>
@@ -2061,7 +2096,7 @@
       </c>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>3</v>
       </c>
@@ -2069,13 +2104,13 @@
         <v>37</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F38" s="6">
         <v>0</v>
@@ -2100,7 +2135,7 @@
       </c>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>3</v>
       </c>
@@ -2108,13 +2143,13 @@
         <v>38</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F39" s="7">
         <v>0</v>
@@ -2139,7 +2174,7 @@
       </c>
       <c r="M39" s="2"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>3</v>
       </c>
@@ -2147,14 +2182,14 @@
         <v>39</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D40" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F40" s="6">
         <v>0</v>
       </c>
@@ -2178,7 +2213,7 @@
       </c>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>3</v>
       </c>
@@ -2186,14 +2221,14 @@
         <v>40</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E41" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F41" s="7">
         <v>0</v>
       </c>
@@ -2217,7 +2252,7 @@
       </c>
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>3</v>
       </c>
@@ -2225,13 +2260,13 @@
         <v>41</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F42" s="6">
         <v>0</v>
@@ -2256,7 +2291,7 @@
       </c>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>3</v>
       </c>
@@ -2264,13 +2299,13 @@
         <v>42</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F43" s="6">
         <v>0</v>
@@ -2295,7 +2330,7 @@
       </c>
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
         <v>3</v>
       </c>
@@ -2303,13 +2338,13 @@
         <v>43</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F44" s="6">
         <v>0</v>
@@ -2334,7 +2369,7 @@
       </c>
       <c r="M44" s="2"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>3</v>
       </c>
@@ -2342,13 +2377,13 @@
         <v>44</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F45" s="6">
         <v>0</v>
@@ -2373,7 +2408,7 @@
       </c>
       <c r="M45" s="2"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>3</v>
       </c>
@@ -2381,13 +2416,13 @@
         <v>45</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F46" s="6">
         <v>0</v>
@@ -2412,7 +2447,7 @@
       </c>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>3</v>
       </c>
@@ -2420,13 +2455,13 @@
         <v>46</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F47" s="7">
         <v>0</v>
@@ -2451,7 +2486,7 @@
       </c>
       <c r="M47" s="2"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>3</v>
       </c>
@@ -2459,13 +2494,13 @@
         <v>47</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F48" s="7">
         <v>0</v>
@@ -2490,7 +2525,7 @@
       </c>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>4</v>
       </c>
@@ -2498,13 +2533,13 @@
         <v>48</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F49" s="7">
         <v>0</v>
@@ -2529,7 +2564,7 @@
       </c>
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>4</v>
       </c>
@@ -2537,13 +2572,13 @@
         <v>49</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F50" s="6">
         <v>0</v>
@@ -2568,7 +2603,7 @@
       </c>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>4</v>
       </c>
@@ -2576,13 +2611,13 @@
         <v>50</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F51" s="6">
         <v>0</v>
@@ -2607,7 +2642,7 @@
       </c>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <v>4</v>
       </c>
@@ -2615,13 +2650,13 @@
         <v>51</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F52" s="6">
         <v>0</v>
@@ -2646,7 +2681,7 @@
       </c>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
         <v>4</v>
       </c>
@@ -2654,13 +2689,13 @@
         <v>52</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F53" s="7">
         <v>0</v>
@@ -2685,7 +2720,7 @@
       </c>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
         <v>4</v>
       </c>
@@ -2693,13 +2728,13 @@
         <v>53</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F54" s="6">
         <v>0</v>
@@ -2724,7 +2759,7 @@
       </c>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
         <v>4</v>
       </c>
@@ -2732,13 +2767,13 @@
         <v>54</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F55" s="7">
         <v>0</v>
@@ -2763,7 +2798,7 @@
       </c>
       <c r="M55" s="2"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
         <v>4</v>
       </c>
@@ -2771,13 +2806,13 @@
         <v>55</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F56" s="7">
         <v>0</v>
@@ -2802,7 +2837,7 @@
       </c>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>4</v>
       </c>
@@ -2810,13 +2845,13 @@
         <v>56</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F57" s="7">
         <v>0</v>
@@ -2841,7 +2876,7 @@
       </c>
       <c r="M57" s="2"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
         <v>4</v>
       </c>
@@ -2849,14 +2884,14 @@
         <v>57</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D58" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F58" s="7">
         <v>0</v>
       </c>
@@ -2880,7 +2915,7 @@
       </c>
       <c r="M58" s="2"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
         <v>4</v>
       </c>
@@ -2888,14 +2923,14 @@
         <v>58</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D59" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F59" s="6">
         <v>0</v>
       </c>
@@ -2919,7 +2954,7 @@
       </c>
       <c r="M59" s="2"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
         <v>4</v>
       </c>
@@ -2927,14 +2962,14 @@
         <v>59</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D60" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E60" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F60" s="6">
         <v>0</v>
       </c>
@@ -2958,7 +2993,7 @@
       </c>
       <c r="M60" s="2"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>4</v>
       </c>
@@ -2966,14 +3001,14 @@
         <v>60</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D61" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E61" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F61" s="7">
         <v>0</v>
       </c>
@@ -2997,7 +3032,7 @@
       </c>
       <c r="M61" s="2"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>4</v>
       </c>
@@ -3005,14 +3040,14 @@
         <v>61</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D62" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E62" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F62" s="7">
         <v>0</v>
       </c>
@@ -3036,7 +3071,7 @@
       </c>
       <c r="M62" s="2"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>4</v>
       </c>
@@ -3044,13 +3079,13 @@
         <v>62</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F63" s="6">
         <v>0</v>
@@ -3075,7 +3110,7 @@
       </c>
       <c r="M63" s="2"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>4</v>
       </c>
@@ -3083,13 +3118,13 @@
         <v>63</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F64" s="6">
         <v>0</v>
@@ -3114,7 +3149,7 @@
       </c>
       <c r="M64" s="2"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <v>4</v>
       </c>
@@ -3122,13 +3157,13 @@
         <v>64</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F65" s="6">
         <v>0</v>
@@ -3153,7 +3188,7 @@
       </c>
       <c r="M65" s="2"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>4</v>
       </c>
@@ -3161,13 +3196,13 @@
         <v>65</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F66" s="7">
         <v>0</v>
@@ -3192,7 +3227,7 @@
       </c>
       <c r="M66" s="2"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
         <v>4</v>
       </c>
@@ -3200,13 +3235,13 @@
         <v>66</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F67" s="6">
         <v>0</v>
@@ -3231,7 +3266,7 @@
       </c>
       <c r="M67" s="2"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
         <v>5</v>
       </c>
@@ -3239,13 +3274,13 @@
         <v>67</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F68" s="6">
         <v>0</v>
@@ -3270,7 +3305,7 @@
       </c>
       <c r="M68" s="2"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
         <v>5</v>
       </c>
@@ -3278,13 +3313,13 @@
         <v>68</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F69" s="6">
         <v>0</v>
@@ -3309,7 +3344,7 @@
       </c>
       <c r="M69" s="2"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
         <v>5</v>
       </c>
@@ -3317,13 +3352,13 @@
         <v>69</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F70" s="6">
         <v>0</v>
@@ -3348,7 +3383,7 @@
       </c>
       <c r="M70" s="2"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>5</v>
       </c>
@@ -3356,13 +3391,13 @@
         <v>70</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F71" s="6">
         <v>0</v>
@@ -3387,7 +3422,7 @@
       </c>
       <c r="M71" s="2"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
         <v>5</v>
       </c>
@@ -3395,13 +3430,13 @@
         <v>71</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F72" s="6">
         <v>0</v>
@@ -3426,7 +3461,7 @@
       </c>
       <c r="M72" s="2"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="11">
         <v>5</v>
       </c>
@@ -3434,13 +3469,13 @@
         <v>72</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F73" s="6">
         <v>0</v>
@@ -3465,7 +3500,7 @@
       </c>
       <c r="M73" s="2"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="11">
         <v>5</v>
       </c>
@@ -3473,13 +3508,13 @@
         <v>73</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F74" s="6">
         <v>0</v>
@@ -3504,7 +3539,7 @@
       </c>
       <c r="M74" s="2"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="11">
         <v>5</v>
       </c>
@@ -3512,13 +3547,13 @@
         <v>74</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F75" s="6">
         <v>0</v>
@@ -3543,7 +3578,7 @@
       </c>
       <c r="M75" s="2"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="11">
         <v>5</v>
       </c>
@@ -3551,13 +3586,13 @@
         <v>75</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F76" s="6">
         <v>0</v>
@@ -3582,7 +3617,7 @@
       </c>
       <c r="M76" s="2"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="11">
         <v>5</v>
       </c>
@@ -3590,13 +3625,13 @@
         <v>76</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F77" s="6">
         <v>0</v>
@@ -3621,7 +3656,7 @@
       </c>
       <c r="M77" s="2"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="11">
         <v>5</v>
       </c>
@@ -3629,13 +3664,13 @@
         <v>77</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F78" s="6">
         <v>0</v>
@@ -3660,7 +3695,7 @@
       </c>
       <c r="M78" s="2"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="11">
         <v>5</v>
       </c>
@@ -3668,14 +3703,14 @@
         <v>78</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D79" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E79" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F79" s="6">
         <v>0</v>
       </c>
@@ -3699,7 +3734,7 @@
       </c>
       <c r="M79" s="2"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="11">
         <v>5</v>
       </c>
@@ -3707,14 +3742,14 @@
         <v>79</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D80" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E80" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E80" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F80" s="6">
         <v>0</v>
       </c>
@@ -3738,7 +3773,7 @@
       </c>
       <c r="M80" s="2"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="11">
         <v>5</v>
       </c>
@@ -3746,14 +3781,14 @@
         <v>80</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D81" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E81" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E81" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F81" s="6">
         <v>0</v>
       </c>
@@ -3777,7 +3812,7 @@
       </c>
       <c r="M81" s="2"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="11">
         <v>5</v>
       </c>
@@ -3785,14 +3820,14 @@
         <v>81</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D82" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E82" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E82" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F82" s="6">
         <v>0</v>
       </c>
@@ -3816,7 +3851,7 @@
       </c>
       <c r="M82" s="2"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="11">
         <v>5</v>
       </c>
@@ -3824,14 +3859,14 @@
         <v>82</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D83" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E83" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E83" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F83" s="6">
         <v>0</v>
       </c>
@@ -3855,7 +3890,7 @@
       </c>
       <c r="M83" s="2"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="11">
         <v>5</v>
       </c>
@@ -3863,14 +3898,14 @@
         <v>83</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D84" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E84" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E84" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F84" s="6">
         <v>0</v>
       </c>
@@ -3894,7 +3929,7 @@
       </c>
       <c r="M84" s="2"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="11">
         <v>5</v>
       </c>
@@ -3902,13 +3937,13 @@
         <v>84</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F85" s="6">
         <v>0</v>
@@ -3933,7 +3968,7 @@
       </c>
       <c r="M85" s="2"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="11">
         <v>5</v>
       </c>
@@ -3941,13 +3976,13 @@
         <v>85</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F86" s="6">
         <v>0</v>
@@ -3972,7 +4007,7 @@
       </c>
       <c r="M86" s="2"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="11">
         <v>5</v>
       </c>
@@ -3980,13 +4015,13 @@
         <v>86</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F87" s="6">
         <v>0</v>
@@ -4011,7 +4046,7 @@
       </c>
       <c r="M87" s="2"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="11">
         <v>5</v>
       </c>
@@ -4019,13 +4054,13 @@
         <v>87</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F88" s="6">
         <v>0</v>
@@ -4050,7 +4085,7 @@
       </c>
       <c r="M88" s="2"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="11">
         <v>5</v>
       </c>
@@ -4058,13 +4093,13 @@
         <v>88</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F89" s="6">
         <v>0</v>
@@ -4089,7 +4124,7 @@
       </c>
       <c r="M89" s="2"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="11">
         <v>6</v>
       </c>
@@ -4097,13 +4132,13 @@
         <v>89</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F90" s="7">
         <v>0</v>
@@ -4128,7 +4163,7 @@
       </c>
       <c r="M90" s="2"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="11">
         <v>6</v>
       </c>
@@ -4136,13 +4171,13 @@
         <v>90</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F91" s="7">
         <v>0</v>
@@ -4167,7 +4202,7 @@
       </c>
       <c r="M91" s="2"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="11">
         <v>6</v>
       </c>
@@ -4175,13 +4210,13 @@
         <v>91</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F92" s="7">
         <v>0</v>
@@ -4206,7 +4241,7 @@
       </c>
       <c r="M92" s="2"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="11">
         <v>6</v>
       </c>
@@ -4214,13 +4249,13 @@
         <v>92</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F93" s="7">
         <v>0</v>
@@ -4245,7 +4280,7 @@
       </c>
       <c r="M93" s="2"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="11">
         <v>6</v>
       </c>
@@ -4253,13 +4288,13 @@
         <v>93</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F94" s="7">
         <v>0</v>
@@ -4284,7 +4319,7 @@
       </c>
       <c r="M94" s="2"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="11">
         <v>6</v>
       </c>
@@ -4292,13 +4327,13 @@
         <v>94</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F95" s="7">
         <v>0</v>
@@ -4323,7 +4358,7 @@
       </c>
       <c r="M95" s="2"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="11">
         <v>6</v>
       </c>
@@ -4331,13 +4366,13 @@
         <v>95</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F96" s="7">
         <v>0</v>
@@ -4362,7 +4397,7 @@
       </c>
       <c r="M96" s="2"/>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="11">
         <v>6</v>
       </c>
@@ -4370,13 +4405,13 @@
         <v>96</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F97" s="7">
         <v>0</v>
@@ -4401,7 +4436,7 @@
       </c>
       <c r="M97" s="2"/>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="11">
         <v>6</v>
       </c>
@@ -4409,13 +4444,13 @@
         <v>97</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F98" s="7">
         <v>0</v>
@@ -4440,7 +4475,7 @@
       </c>
       <c r="M98" s="2"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="11">
         <v>6</v>
       </c>
@@ -4448,13 +4483,13 @@
         <v>98</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F99" s="7">
         <v>0</v>
@@ -4479,7 +4514,7 @@
       </c>
       <c r="M99" s="2"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="11">
         <v>6</v>
       </c>
@@ -4487,13 +4522,13 @@
         <v>99</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F100" s="7">
         <v>0</v>
@@ -4518,7 +4553,7 @@
       </c>
       <c r="M100" s="2"/>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="11">
         <v>6</v>
       </c>
@@ -4526,13 +4561,13 @@
         <v>100</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F101" s="7">
         <v>0</v>
@@ -4557,7 +4592,7 @@
       </c>
       <c r="M101" s="2"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="11">
         <v>6</v>
       </c>
@@ -4565,13 +4600,13 @@
         <v>101</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F102" s="7">
         <v>0</v>
@@ -4596,7 +4631,7 @@
       </c>
       <c r="M102" s="2"/>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="11">
         <v>6</v>
       </c>
@@ -4604,13 +4639,13 @@
         <v>102</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F103" s="7">
         <v>0</v>
@@ -4635,7 +4670,7 @@
       </c>
       <c r="M103" s="2"/>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="11">
         <v>6</v>
       </c>
@@ -4643,14 +4678,14 @@
         <v>103</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D104" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E104" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E104" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F104" s="7">
         <v>0</v>
       </c>
@@ -4674,7 +4709,7 @@
       </c>
       <c r="M104" s="2"/>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="11">
         <v>6</v>
       </c>
@@ -4682,14 +4717,14 @@
         <v>104</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D105" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E105" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E105" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F105" s="7">
         <v>0</v>
       </c>
@@ -4713,7 +4748,7 @@
       </c>
       <c r="M105" s="2"/>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="11">
         <v>6</v>
       </c>
@@ -4721,14 +4756,14 @@
         <v>105</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D106" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E106" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E106" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F106" s="7">
         <v>0</v>
       </c>
@@ -4752,7 +4787,7 @@
       </c>
       <c r="M106" s="2"/>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="11">
         <v>6</v>
       </c>
@@ -4760,14 +4795,14 @@
         <v>106</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D107" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E107" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E107" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F107" s="7">
         <v>0</v>
       </c>
@@ -4791,7 +4826,7 @@
       </c>
       <c r="M107" s="2"/>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="11">
         <v>6</v>
       </c>
@@ -4799,14 +4834,14 @@
         <v>107</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D108" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E108" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E108" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F108" s="7">
         <v>0</v>
       </c>
@@ -4830,7 +4865,7 @@
       </c>
       <c r="M108" s="2"/>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="11">
         <v>6</v>
       </c>
@@ -4838,14 +4873,14 @@
         <v>108</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D109" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E109" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E109" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F109" s="7">
         <v>0</v>
       </c>
@@ -4869,7 +4904,7 @@
       </c>
       <c r="M109" s="2"/>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="11">
         <v>6</v>
       </c>
@@ -4877,14 +4912,14 @@
         <v>109</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D110" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E110" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E110" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F110" s="7">
         <v>0</v>
       </c>
@@ -4908,7 +4943,7 @@
       </c>
       <c r="M110" s="2"/>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="11">
         <v>6</v>
       </c>
@@ -4916,14 +4951,14 @@
         <v>110</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D111" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E111" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E111" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F111" s="7">
         <v>0</v>
       </c>
@@ -4947,7 +4982,7 @@
       </c>
       <c r="M111" s="2"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="11">
         <v>6</v>
       </c>
@@ -4955,13 +4990,13 @@
         <v>111</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F112" s="7">
         <v>0</v>
@@ -4986,7 +5021,7 @@
       </c>
       <c r="M112" s="2"/>
     </row>
-    <row r="113" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A113" s="11">
         <v>6</v>
       </c>
@@ -4994,13 +5029,13 @@
         <v>112</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F113" s="7">
         <v>0</v>
@@ -5025,7 +5060,7 @@
       </c>
       <c r="M113" s="2"/>
     </row>
-    <row r="114" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A114" s="11">
         <v>6</v>
       </c>
@@ -5033,13 +5068,13 @@
         <v>113</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F114" s="7">
         <v>0</v>
@@ -5064,7 +5099,7 @@
       </c>
       <c r="M114" s="2"/>
     </row>
-    <row r="115" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A115" s="11">
         <v>6</v>
       </c>
@@ -5072,13 +5107,13 @@
         <v>114</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F115" s="7">
         <v>0</v>
@@ -5103,7 +5138,7 @@
       </c>
       <c r="M115" s="2"/>
     </row>
-    <row r="116" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A116" s="11">
         <v>6</v>
       </c>
@@ -5111,13 +5146,13 @@
         <v>115</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F116" s="7">
         <v>0</v>
@@ -5142,7 +5177,7 @@
       </c>
       <c r="M116" s="2"/>
     </row>
-    <row r="117" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A117" s="11">
         <v>6</v>
       </c>
@@ -5150,13 +5185,13 @@
         <v>116</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F117" s="7">
         <v>0</v>
@@ -5181,7 +5216,7 @@
       </c>
       <c r="M117" s="2"/>
     </row>
-    <row r="118" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A118" s="11">
         <v>7</v>
       </c>
@@ -5189,13 +5224,13 @@
         <v>117</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F118" s="7">
         <v>0</v>
@@ -5220,7 +5255,7 @@
       </c>
       <c r="M118" s="2"/>
     </row>
-    <row r="119" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A119" s="11">
         <v>7</v>
       </c>
@@ -5228,13 +5263,13 @@
         <v>118</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F119" s="7">
         <v>0</v>
@@ -5259,7 +5294,7 @@
       </c>
       <c r="M119" s="2"/>
     </row>
-    <row r="120" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A120" s="11">
         <v>7</v>
       </c>
@@ -5267,13 +5302,13 @@
         <v>119</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F120" s="7">
         <v>0</v>
@@ -5298,7 +5333,7 @@
       </c>
       <c r="M120" s="2"/>
     </row>
-    <row r="121" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A121" s="11">
         <v>7</v>
       </c>
@@ -5306,13 +5341,13 @@
         <v>120</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F121" s="7">
         <v>0</v>
@@ -5337,7 +5372,7 @@
       </c>
       <c r="M121" s="2"/>
     </row>
-    <row r="122" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A122" s="11">
         <v>7</v>
       </c>
@@ -5345,13 +5380,13 @@
         <v>121</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F122" s="7">
         <v>0</v>
@@ -5376,7 +5411,7 @@
       </c>
       <c r="M122" s="2"/>
     </row>
-    <row r="123" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A123" s="11">
         <v>7</v>
       </c>
@@ -5384,13 +5419,13 @@
         <v>122</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F123" s="7">
         <v>0</v>
@@ -5415,7 +5450,7 @@
       </c>
       <c r="M123" s="2"/>
     </row>
-    <row r="124" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A124" s="11">
         <v>7</v>
       </c>
@@ -5423,13 +5458,13 @@
         <v>123</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F124" s="7">
         <v>0</v>
@@ -5454,7 +5489,7 @@
       </c>
       <c r="M124" s="2"/>
     </row>
-    <row r="125" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A125" s="11">
         <v>7</v>
       </c>
@@ -5462,13 +5497,13 @@
         <v>124</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F125" s="7">
         <v>0</v>
@@ -5534,7 +5569,7 @@
       <c r="BG125" s="4"/>
       <c r="BH125" s="4"/>
     </row>
-    <row r="126" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A126" s="11">
         <v>7</v>
       </c>
@@ -5542,13 +5577,13 @@
         <v>125</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F126" s="7">
         <v>0</v>
@@ -5614,7 +5649,7 @@
       <c r="BG126" s="4"/>
       <c r="BH126" s="4"/>
     </row>
-    <row r="127" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A127" s="11">
         <v>7</v>
       </c>
@@ -5622,14 +5657,14 @@
         <v>126</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D127" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E127" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E127" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F127" s="7">
         <v>0</v>
       </c>
@@ -5653,7 +5688,7 @@
       </c>
       <c r="AF127" s="2"/>
     </row>
-    <row r="128" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A128" s="11">
         <v>7</v>
       </c>
@@ -5661,13 +5696,13 @@
         <v>127</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D128" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E128" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="E128" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="F128" s="7">
         <v>0</v>
@@ -5701,7 +5736,7 @@
       <c r="AZ128" s="3"/>
       <c r="BA128" s="3"/>
     </row>
-    <row r="129" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A129" s="11">
         <v>7</v>
       </c>
@@ -5709,14 +5744,14 @@
         <v>128</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D129" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E129" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E129" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F129" s="7">
         <v>0</v>
       </c>
@@ -5740,7 +5775,7 @@
       </c>
       <c r="AF129" s="2"/>
     </row>
-    <row r="130" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A130" s="11">
         <v>7</v>
       </c>
@@ -5748,13 +5783,13 @@
         <v>129</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D130" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E130" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="E130" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="F130" s="7">
         <v>0</v>
@@ -5802,7 +5837,7 @@
       <c r="BF130" s="3"/>
       <c r="BG130" s="3"/>
     </row>
-    <row r="131" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A131" s="11">
         <v>7</v>
       </c>
@@ -5810,13 +5845,13 @@
         <v>130</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F131" s="7">
         <v>0</v>
@@ -5840,7 +5875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A132" s="11">
         <v>7</v>
       </c>
@@ -5848,13 +5883,13 @@
         <v>131</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F132" s="7">
         <v>0</v>
@@ -5878,7 +5913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A133" s="11">
         <v>7</v>
       </c>
@@ -5886,13 +5921,13 @@
         <v>132</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F133" s="7">
         <v>0</v>

</xml_diff>